<commit_message>
Adds traceability for factory
</commit_message>
<xml_diff>
--- a/SoftEngMidterm/SoftEngMidterm/traceability.xlsx
+++ b/SoftEngMidterm/SoftEngMidterm/traceability.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dragon\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Bridge Traceability</t>
   </si>
@@ -156,25 +161,40 @@
     <t xml:space="preserve"> iteratorTest</t>
   </si>
   <si>
-    <t xml:space="preserve"> Factory.java: lines 5-42</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Factory.cs all (modification to generate an object each time instead of passing a reference to the same object each time)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> no change necessary to factory test class</t>
-  </si>
-  <si>
     <t>Iterator Traceability</t>
   </si>
   <si>
     <t>Factory Traceability</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>T12, T13</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>J16</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>T12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -192,7 +212,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -200,20 +220,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -538,23 +623,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" customHeight="1">
+    <row r="1" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -565,7 +655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -576,7 +666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -587,7 +677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -598,7 +688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -609,7 +699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -620,7 +710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -631,7 +721,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -642,7 +732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -653,7 +743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -664,7 +754,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -675,7 +765,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -686,69 +776,112 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C21" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A23:C23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Total time for student 2: 3h 30 min -itter trace
</commit_message>
<xml_diff>
--- a/SoftEngMidterm/SoftEngMidterm/traceability.xlsx
+++ b/SoftEngMidterm/SoftEngMidterm/traceability.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dragon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dillon\Desktop\git\noreqsjustdeliver\SoftEngMidterm\SoftEngMidterm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
   <si>
     <t>Bridge Traceability</t>
   </si>
@@ -189,12 +189,99 @@
   </si>
   <si>
     <t>T12</t>
+  </si>
+  <si>
+    <t>J17</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>J18</t>
+  </si>
+  <si>
+    <t>J19</t>
+  </si>
+  <si>
+    <t>J20</t>
+  </si>
+  <si>
+    <t>J21</t>
+  </si>
+  <si>
+    <t>J22</t>
+  </si>
+  <si>
+    <t>J23</t>
+  </si>
+  <si>
+    <t>J24</t>
+  </si>
+  <si>
+    <t>J25</t>
+  </si>
+  <si>
+    <t>J26</t>
+  </si>
+  <si>
+    <t>J27</t>
+  </si>
+  <si>
+    <t>J28</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>T14, T15, T16, T17, T18, T19</t>
+  </si>
+  <si>
+    <t>T14, T15, T16, T17</t>
+  </si>
+  <si>
+    <t>T16, T17</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <t>T18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -278,13 +365,13 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,11 +710,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -638,243 +725,386 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>